<commit_message>
Ispravljen AN za asistente (header predavanje/rac)
</commit_message>
<xml_diff>
--- a/Novi_Izveštaj o radu_za_Nastavnike_Natasa_Bogdanovic - Copy.xlsx
+++ b/Novi_Izveštaj o radu_za_Nastavnike_Natasa_Bogdanovic - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtsnis-my.sharepoint.com/personal/milan_ristic_akademijanis_edu_rs/Documents/Git folder za generator radnih svezaka/GeneratorRadnihSvezaka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{515AE231-9F81-4BD4-8A77-B049EAC38BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9EF8748-4874-4A4E-8D75-8FF2E5E65546}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{515AE231-9F81-4BD4-8A77-B049EAC38BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{171A80ED-F3B7-46E7-8565-0D4FC2FE0270}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{63FCCB33-4A62-4BAF-94D7-AE2680D11626}"/>
   </bookViews>
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2541,16 +2541,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -2982,6 +2973,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Excel Services" refreshedDate="45700.930710995373" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="460" xr:uid="{530C62FA-8687-4493-BDAF-577F166D3B65}">
   <cacheSource type="worksheet">
@@ -7700,201 +7695,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86524379-27E0-4EB7-B6B8-D950279E7120}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Predmeti">
-  <location ref="C29:D48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField numFmtId="14" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <items count="29">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="28"/>
-        <item x="10"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <items count="2">
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="1"/>
-    <field x="9"/>
-    <field x="8"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="19">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Prosečan broj studenata" fld="7" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0F9F3DAC-0054-4948-AFB7-521DAFF30AAA}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Predmeti" colHeaderCaption="Vrsta nastave">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0F9F3DAC-0054-4948-AFB7-521DAFF30AAA}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Predmeti" colHeaderCaption="Vrsta nastave">
   <location ref="B6:E26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="14" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -8074,18 +7875,212 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86524379-27E0-4EB7-B6B8-D950279E7120}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Predmeti">
+  <location ref="J6:K25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField numFmtId="14" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="29">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="28"/>
+        <item x="10"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="1"/>
+    <field x="9"/>
+    <field x="8"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Prosečan broj studenata" fld="7" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16781676-077F-4238-A45B-27DFF94B5076}" name="evidencija_nastave" displayName="evidencija_nastave" ref="A1:H461" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16781676-077F-4238-A45B-27DFF94B5076}" name="evidencija_nastave" displayName="evidencija_nastave" ref="A1:H461" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:H461" xr:uid="{16781676-077F-4238-A45B-27DFF94B5076}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{50194762-F77D-4094-AA6D-99EE30260FD4}" name="Datum " dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{0C577E04-68A0-4F23-BA45-D6CB7CBDAEF9}" name="Odsek" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7FB038C7-1C51-4E8D-89D6-40EFCD2C3E30}" name="Studijski program" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{42258C3E-B96F-493F-9BC3-C4653A46D16E}" name="Predmet" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{D2E1579F-AC74-46B0-A298-2A297A6F019C}" name="Tip nastave" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{10597A3E-1A4A-4D17-B23F-3033813457E5}" name="Broj časova nastave" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{3E5CD073-EB68-4D84-93A7-166020BE5AA0}" name="Nastavna jedinica" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{9FC5B2DF-EA47-4EFD-A8D3-B4CCE22F5F1B}" name="Broj prisutnih studenata" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{50194762-F77D-4094-AA6D-99EE30260FD4}" name="Datum " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{0C577E04-68A0-4F23-BA45-D6CB7CBDAEF9}" name="Odsek" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7FB038C7-1C51-4E8D-89D6-40EFCD2C3E30}" name="Studijski program" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{42258C3E-B96F-493F-9BC3-C4653A46D16E}" name="Predmet" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{D2E1579F-AC74-46B0-A298-2A297A6F019C}" name="Tip nastave" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{10597A3E-1A4A-4D17-B23F-3033813457E5}" name="Broj časova nastave" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{3E5CD073-EB68-4D84-93A7-166020BE5AA0}" name="Nastavna jedinica" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{9FC5B2DF-EA47-4EFD-A8D3-B4CCE22F5F1B}" name="Broj prisutnih studenata" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15820,10 +15815,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB64B95-66F9-4F12-9234-061A62D7269E}">
-  <dimension ref="A4:F48"/>
+  <dimension ref="A4:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="108" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15842,7 +15837,7 @@
     <col min="12" max="12" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
@@ -15850,7 +15845,7 @@
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="61" t="s">
         <v>196</v>
       </c>
@@ -15859,8 +15854,14 @@
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="63"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J6" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="K6" s="66" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="61" t="s">
         <v>198</v>
       </c>
@@ -15873,32 +15874,50 @@
       <c r="E7" s="66" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J7" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="67" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="64"/>
       <c r="D8" s="65"/>
       <c r="E8" s="66"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J8" s="68" t="s">
+        <v>202</v>
+      </c>
+      <c r="K8" s="80"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="68" t="s">
         <v>202</v>
       </c>
       <c r="C9" s="69"/>
       <c r="D9" s="70"/>
       <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J9" s="72" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="72" t="s">
         <v>204</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" s="70"/>
       <c r="E10" s="71"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J10" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="73" t="s">
         <v>16</v>
       </c>
@@ -15911,8 +15930,14 @@
       <c r="E11" s="71">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J11" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="80">
+        <v>11.333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="73" t="s">
         <v>59</v>
       </c>
@@ -15925,24 +15950,38 @@
       <c r="E12" s="71">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J12" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="K12" s="80"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="68" t="s">
         <v>203</v>
       </c>
       <c r="C13" s="69"/>
       <c r="D13" s="70"/>
       <c r="E13" s="71"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J13" s="72" t="s">
+        <v>205</v>
+      </c>
+      <c r="K13" s="80"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="72" t="s">
         <v>205</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="70"/>
       <c r="E14" s="71"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J14" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="80">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="73" t="s">
         <v>16</v>
       </c>
@@ -15953,8 +15992,14 @@
       <c r="E15" s="71">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J15" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="80">
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="73" t="s">
         <v>59</v>
       </c>
@@ -15965,16 +16010,26 @@
       <c r="E16" s="71">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J16" s="72" t="s">
+        <v>206</v>
+      </c>
+      <c r="K16" s="80"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="72" t="s">
         <v>206</v>
       </c>
       <c r="C17" s="69"/>
       <c r="D17" s="70"/>
       <c r="E17" s="71"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J17" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="80">
+        <v>30.75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="73" t="s">
         <v>16</v>
       </c>
@@ -15987,8 +16042,14 @@
       <c r="E18" s="71">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J18" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" s="80">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="73" t="s">
         <v>59</v>
       </c>
@@ -16001,16 +16062,26 @@
       <c r="E19" s="71">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J19" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="K19" s="80"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="72" t="s">
         <v>207</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="70"/>
       <c r="E20" s="71"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J20" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="80">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="73" t="s">
         <v>16</v>
       </c>
@@ -16021,8 +16092,14 @@
       <c r="E21" s="71">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J21" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="80">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="73" t="s">
         <v>59</v>
       </c>
@@ -16033,176 +16110,54 @@
       <c r="E22" s="71">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J22" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="K22" s="80"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="74" t="s">
         <v>200</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="70"/>
       <c r="E23" s="71"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J23" s="68" t="s">
+        <v>595</v>
+      </c>
+      <c r="K23" s="80"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="68" t="s">
         <v>595</v>
       </c>
       <c r="C24" s="69"/>
       <c r="D24" s="70"/>
       <c r="E24" s="71"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J24" s="72" t="s">
+        <v>595</v>
+      </c>
+      <c r="K24" s="80"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="72" t="s">
         <v>595</v>
       </c>
       <c r="C25" s="69"/>
       <c r="D25" s="70"/>
       <c r="E25" s="71"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J25" s="75" t="s">
+        <v>200</v>
+      </c>
+      <c r="K25" s="81"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="75" t="s">
         <v>200</v>
       </c>
       <c r="C26" s="76"/>
       <c r="D26" s="77"/>
       <c r="E26" s="78"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="61" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="66" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="79"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="68" t="s">
-        <v>202</v>
-      </c>
-      <c r="D31" s="80"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="72" t="s">
-        <v>204</v>
-      </c>
-      <c r="D32" s="80"/>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C33" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="80">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C34" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="80">
-        <v>11.333333333333334</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="68" t="s">
-        <v>203</v>
-      </c>
-      <c r="D35" s="80"/>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C36" s="72" t="s">
-        <v>205</v>
-      </c>
-      <c r="D36" s="80"/>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C37" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="80">
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C38" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="80">
-        <v>32.75</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C39" s="72" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="80"/>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C40" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="80">
-        <v>30.75</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C41" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="80">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C42" s="72" t="s">
-        <v>207</v>
-      </c>
-      <c r="D42" s="80"/>
-    </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C43" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="80">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C44" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="80">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C45" s="74" t="s">
-        <v>200</v>
-      </c>
-      <c r="D45" s="80"/>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C46" s="68" t="s">
-        <v>595</v>
-      </c>
-      <c r="D46" s="80"/>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C47" s="72" t="s">
-        <v>595</v>
-      </c>
-      <c r="D47" s="80"/>
-    </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C48" s="75" t="s">
-        <v>200</v>
-      </c>
-      <c r="D48" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>